<commit_message>
day03 part 1 and day04
</commit_message>
<xml_diff>
--- a/spiral_test_day03.xlsx
+++ b/spiral_test_day03.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FGiordano-Silva\DataAnalyst\Python\advent2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B10E2EA-7B18-419E-8372-C4427BF71DED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB16B80-9665-4FA1-A42A-56BB155F290A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A3FD0C0F-6479-4AB0-BEC6-70F306506BFF}"/>
+    <workbookView xWindow="195" yWindow="16935" windowWidth="20490" windowHeight="10920" xr2:uid="{A3FD0C0F-6479-4AB0-BEC6-70F306506BFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>What is the coordenate</t>
   </si>
@@ -112,13 +112,19 @@
   </si>
   <si>
     <t>(2, -1)</t>
+  </si>
+  <si>
+    <t>whats the odd square</t>
+  </si>
+  <si>
+    <t>odd_square</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,8 +138,32 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +182,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -165,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -179,6 +215,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,13 +536,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29E27A4-95EB-447C-AE46-674C487AD0B9}">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" customWidth="1"/>
   </cols>
@@ -511,7 +553,9 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="K2" s="6"/>
+      <c r="K2" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="L2" s="6" t="s">
         <v>6</v>
       </c>
@@ -537,7 +581,9 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
-      <c r="K3" s="7"/>
+      <c r="K3" s="7">
+        <v>1</v>
+      </c>
       <c r="L3" s="6" t="s">
         <v>7</v>
       </c>
@@ -565,7 +611,9 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="7"/>
+      <c r="K4" s="7">
+        <v>3</v>
+      </c>
       <c r="L4" s="6" t="s">
         <v>8</v>
       </c>
@@ -611,7 +659,9 @@
         <v>57</v>
       </c>
       <c r="J5" s="4"/>
-      <c r="K5" s="7"/>
+      <c r="K5" s="7">
+        <v>5</v>
+      </c>
       <c r="L5" s="6" t="s">
         <v>9</v>
       </c>
@@ -632,25 +682,25 @@
       <c r="A6" s="4">
         <v>66</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="9">
         <v>37</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="9">
         <v>36</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="9">
         <v>35</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="9">
         <v>34</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="9">
         <v>33</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="9">
         <v>32</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="9">
         <v>31</v>
       </c>
       <c r="I6" s="4">
@@ -678,25 +728,25 @@
       <c r="A7" s="4">
         <v>67</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="9">
         <v>38</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="9">
         <v>17</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="9">
         <v>16</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="9">
         <v>15</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="9">
         <v>14</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="9">
         <v>13</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="9">
         <v>30</v>
       </c>
       <c r="I7" s="4">
@@ -724,25 +774,25 @@
       <c r="A8" s="4">
         <v>68</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="9">
         <v>39</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="9">
         <v>18</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="9">
         <v>5</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="9">
         <v>4</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="9">
         <v>3</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="9">
         <v>12</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="9">
         <v>29</v>
       </c>
       <c r="I8" s="4">
@@ -762,25 +812,25 @@
       <c r="A9" s="4">
         <v>69</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="9">
         <v>40</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="9">
         <v>19</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="9">
         <v>6</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="10">
         <v>1</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="9">
         <v>2</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="9">
         <v>11</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="9">
         <v>28</v>
       </c>
       <c r="I9" s="4">
@@ -800,25 +850,25 @@
       <c r="A10" s="4">
         <v>70</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="9">
         <v>41</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="9">
         <v>20</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="9">
         <v>7</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="9">
         <v>8</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="10">
         <v>9</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="9">
         <v>10</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="9">
         <v>27</v>
       </c>
       <c r="I10" s="4">
@@ -847,25 +897,25 @@
       <c r="A11" s="4">
         <v>71</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="9">
         <v>42</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="9">
         <v>21</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="9">
         <v>22</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="9">
         <v>23</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="9">
         <v>24</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="10">
         <v>25</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="11">
         <v>26</v>
       </c>
       <c r="I11" s="4">
@@ -881,32 +931,32 @@
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>72</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="9">
         <v>43</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="12">
         <v>44</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="12">
         <v>45</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="12">
         <v>46</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="12">
         <v>47</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="13">
         <v>48</v>
       </c>
       <c r="H12" s="2">
         <v>49</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="4">
         <v>50</v>
       </c>
       <c r="J12" s="4"/>
@@ -947,7 +997,7 @@
       <c r="I13" s="2">
         <v>81</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="4">
         <v>82</v>
       </c>
       <c r="K13" s="7"/>
@@ -1003,23 +1053,7 @@
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
       <c r="E19" s="4">
         <v>5</v>
       </c>
@@ -1030,7 +1064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
       <c r="E20" s="4">
         <v>6</v>
       </c>
@@ -1041,7 +1075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
       <c r="E21" s="4">
         <v>7</v>
       </c>
@@ -1051,8 +1085,22 @@
       <c r="G21" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>12</v>
       </c>
@@ -1062,8 +1110,14 @@
       <c r="E23" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="M23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>7</v>
       </c>
@@ -1071,7 +1125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>16</v>
       </c>
@@ -1082,7 +1136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>8</v>
       </c>
@@ -1093,7 +1147,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>20</v>
       </c>
@@ -1104,7 +1158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>21</v>
       </c>
@@ -1115,7 +1169,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>22</v>
       </c>
@@ -1126,7 +1180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>23</v>
       </c>
@@ -1137,7 +1191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>24</v>
       </c>
@@ -1148,7 +1202,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>25</v>
       </c>

</xml_diff>